<commit_message>
updated journal and README.md, added new images and BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/58d29176c16c150d/my stuff/RC Boat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4CCD472-029B-420E-87EA-C64C627BB8BD}"/>
+  <xr:revisionPtr revIDLastSave="312" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FED6907-FE2D-475B-A9CB-3AA815FE8747}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="0" windowWidth="20505" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
   <si>
     <t>Item</t>
   </si>
@@ -44,33 +44,54 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Delivery</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Pololu 19:1 Metal Gearmotor 37Dx52L mm 12V</t>
-  </si>
-  <si>
-    <t>Robot Shop</t>
-  </si>
-  <si>
-    <t>Pololu 19:1 Metal Gearmotor 37Dx52L mm 12V (Helical Pinion) - RobotShop</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>12V 775 motor</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>EsportsMJJ 775 Motor DC 12V-36V 3500-9000RPM Motor Large Torque High-power Motor : Amazon.co.uk: Automotive</t>
+  </si>
+  <si>
+    <t>motor to drive to prop</t>
+  </si>
+  <si>
+    <t>helping hands</t>
+  </si>
+  <si>
+    <t>aliexpress</t>
+  </si>
+  <si>
+    <t>Toolour Soldering Station Helping Hand Third Hand Tool 3/4/5 Flexible Arms with Adjustable Vise Table Desk Clamp Base PCB Holder - AliExpress</t>
   </si>
   <si>
     <t>BTS7960 Motor Driver Module</t>
   </si>
   <si>
-    <t>amazon</t>
-  </si>
-  <si>
     <t>Hailege BTS7960 43A Dual H-Bridge Stepper Motor Drive Current Limit Control Semiconductor Refrigeration PWM for Smart Car Motor Drive : Amazon.co.uk: Business, Industry &amp; Science</t>
   </si>
   <si>
+    <t>driver to control the power of the motor through Pi PWM</t>
+  </si>
+  <si>
+    <t>lipo battery charger</t>
+  </si>
+  <si>
+    <t>iMAX B6 V3 80W 6A Battery Charger LiHv Lipo NiMh Li-ion Ni-Cd Digital RC Charger Lipro Balance Charger Discharger 15V 6A Adapter - AliExpress</t>
+  </si>
+  <si>
+    <t>to charge the battery</t>
+  </si>
+  <si>
     <t>Pololu 5V D24V5F5</t>
   </si>
   <si>
@@ -80,7 +101,16 @@
     <t>Pololu 5V, 500mA Step-Down Voltage Regulator D24V5F5 - RangeVideo</t>
   </si>
   <si>
-    <t>aliexpress</t>
+    <t>step down converter from 11.1V battery, to 5V for the Pi and servo</t>
+  </si>
+  <si>
+    <t>ky040</t>
+  </si>
+  <si>
+    <t>5pcs 360 Degree Rotary Encoder Module KY-040 Brick Sensor Development Board with 15 X 16.5 Mm Buttons for Arduino - AliExpress</t>
+  </si>
+  <si>
+    <t>hoping this will work on the secondary pi to control the boat</t>
   </si>
   <si>
     <t>5 pair plug</t>
@@ -92,7 +122,16 @@
     <t>XT60 XT-60 Male Female Bullet Connectors Plugs With Silicon 14 AWG Wire For RC Lipo Battery Quadcopter Multicopter Hot Sale - AliExpress</t>
   </si>
   <si>
-    <t>other</t>
+    <t>Battery connectors</t>
+  </si>
+  <si>
+    <t>isopropyl</t>
+  </si>
+  <si>
+    <t>Tech Grade Isopropanol Alcohol IPA 99.99% (500ml Spray) : Amazon.co.uk: Business, Industry &amp; Science</t>
+  </si>
+  <si>
+    <t>cleaning solder</t>
   </si>
   <si>
     <t>1-Male to 2-Female XT60</t>
@@ -101,6 +140,18 @@
     <t>XT60 Male Female 3-Way Parallel Connector 14AWG High Current Silicone Wire Y Splitter for Battery Charger Motor Drone RC Models - AliExpress</t>
   </si>
   <si>
+    <t xml:space="preserve">battery splitter </t>
+  </si>
+  <si>
+    <t>rudder</t>
+  </si>
+  <si>
+    <t>1 Pcs RC Boat Aluminium Alloy Brand New 75mm 95mm Metal Suction Water Rudder For Remote Control RC Boats CNC Upgrade Parts - AliExpress 26</t>
+  </si>
+  <si>
+    <t>rudder kit.</t>
+  </si>
+  <si>
     <t>ZOP POWER 11.1V 1500mAh 45C 3S LiPo Battery </t>
   </si>
   <si>
@@ -110,39 +161,123 @@
     <t>ZOP POWER 11.1V 1500mAh 45C 3S LiPo Battery XT60 Plug for RC Drone Sale - Banggood UK</t>
   </si>
   <si>
+    <t>11.1V battery with enough power for the 12V motor and capacity for a good 10-20 minutes</t>
+  </si>
+  <si>
+    <t>motor couple 3.17-6mm</t>
+  </si>
+  <si>
+    <t>2mm/3mm/3.17mm/4mm/5mm/6mm/6.35mm/7mm/8mm/10mm Aluminum Rigid Shaft Coupler Rigid Coupling Motor Connector - AliExpress 13</t>
+  </si>
+  <si>
+    <t>connect the motor to the drive shaft</t>
+  </si>
+  <si>
     <t>18AWG wire</t>
   </si>
   <si>
     <t>2-pin red and black PVC or silicone extension cable 28awg 26awg 24awg 22awg 20awg 18awg 16awg Tinned copper domestic wire - AliExpress 13</t>
   </si>
   <si>
+    <t>thicker wire for battery connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glue  </t>
+  </si>
+  <si>
+    <t>Plastic Glue 30 g, Clear Model Glue, Superglue for Plastic, Acrylic, Model, 3D Printing, Miniatures, PVC, Vinyl, with Anti-Clog Cap, Waterproof, Heat-Resistant : Amazon.co.uk: Home &amp; Kitchen</t>
+  </si>
+  <si>
+    <t>superglue for everything</t>
+  </si>
+  <si>
     <t>1 pair female male</t>
   </si>
   <si>
+    <t>more battery connectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expanding foam </t>
+  </si>
+  <si>
+    <t>500ml Gap Expanding Foam Filler PU Expansion Insulation BONDING Filling - 1x : Amazon.co.uk: DIY &amp; Tools</t>
+  </si>
+  <si>
+    <t>not sure if this is needed in my 3d model to help it float but safe to put it here anyway</t>
+  </si>
+  <si>
     <t>nRF24L01 x5</t>
   </si>
   <si>
     <t>1-10pcs NRF24L01+PA+LNA 2.4G Wireless Module 1100-Meter Long-Distance With Antenna - AliExpress</t>
   </si>
   <si>
+    <t>2.4GHz RF modules for communications between Pis</t>
+  </si>
+  <si>
+    <t>prop set</t>
+  </si>
+  <si>
+    <t>1set 3.17mm 1/8" Flexible Cable Shaft + Shaft Sleeve + Mount Holder + 32mm Propeller Kit for RC Boats Marine Yacht - AliExpress 26</t>
+  </si>
+  <si>
+    <t>shaft and propeller</t>
+  </si>
+  <si>
     <t>solder tweezers</t>
   </si>
   <si>
     <t>6Pcs Anti-static ESD Stainless Steel Tweezers Maintenance Tool Industrial Precision Curved Straight Tweezers Repair Tools Set - AliExpress 34</t>
   </si>
   <si>
+    <t>yeah pretty self explanatory</t>
+  </si>
+  <si>
+    <t>0.1-10uF caps</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/KYOCERA-AVX/SA305C104KARC?qs=sGAEpiMZZMuMW9TJLBQkXkxKN5DNfsrexST853eVphY%3D</t>
+  </si>
+  <si>
+    <t>capacitors</t>
+  </si>
+  <si>
     <t>heat shrink tubing</t>
   </si>
   <si>
     <t>254/270pcs 3X Shrink Tape Glue Red And Black, Heat Shrinkable Tube Box Heat Shrink Tube Combined With Heat Shrink Insulation - AliExpress</t>
   </si>
   <si>
+    <t>safety first!</t>
+  </si>
+  <si>
+    <t>electolytic caps</t>
+  </si>
+  <si>
+    <t>860010474013 Wurth Elektronik | Mouser United Kingdom</t>
+  </si>
+  <si>
     <t>wire strippers</t>
   </si>
   <si>
     <t>Amazon Basics Self-Adjusting Wire Stripper, Black/red : Amazon.co.uk: DIY &amp; Tools</t>
   </si>
   <si>
+    <t>10k resistor</t>
+  </si>
+  <si>
+    <t>rapidelectronics</t>
+  </si>
+  <si>
+    <t>https://www.rapidonline.com/10k-0-25w-royal-ohm-metal-film-resistor-100pc-cut-tape-62-3474</t>
+  </si>
+  <si>
+    <t>resistors</t>
+  </si>
+  <si>
     <t>XTC-3D</t>
   </si>
   <si>
@@ -152,64 +287,43 @@
     <t>3D Printers, Filament &amp; Tools | Best prices UK | 123-3d.co.uk</t>
   </si>
   <si>
+    <t>epoxy for sealing the 3D print</t>
+  </si>
+  <si>
+    <t>47 resistor</t>
+  </si>
+  <si>
+    <t>https://www.rapidonline.com/47r-0-25w-royal-ohm-metal-film-resistor-100pc-cut-tape-62-3418</t>
+  </si>
+  <si>
     <t>glue gun</t>
   </si>
   <si>
     <t>Tilswall Hot Glue Gun Kit, 50W Mini Melt Gun with 75pcs 130mm Glue Sticks for Crafting, DIY, Art, Sealing, Home Repairs, Cards, and Glass : Amazon.co.uk: DIY &amp; Tools</t>
   </si>
   <si>
-    <t>helping hands</t>
-  </si>
-  <si>
-    <t>Toolour Soldering Station Helping Hand Third Hand Tool 3/4/5 Flexible Arms with Adjustable Vise Table Desk Clamp Base PCB Holder - AliExpress</t>
-  </si>
-  <si>
-    <t>lipo battery charger</t>
-  </si>
-  <si>
-    <t>iMAX B6 V3 80W 6A Battery Charger LiHv Lipo NiMh Li-ion Ni-Cd Digital RC Charger Lipro Balance Charger Discharger 15V 6A Adapter - AliExpress</t>
-  </si>
-  <si>
-    <t>ky040</t>
-  </si>
-  <si>
-    <t>5pcs 360 Degree Rotary Encoder Module KY-040 Brick Sensor Development Board with 15 X 16.5 Mm Buttons for Arduino - AliExpress</t>
-  </si>
-  <si>
-    <t>isopropyl</t>
-  </si>
-  <si>
-    <t>Tech Grade Isopropanol Alcohol IPA 99.99% (500ml Spray) : Amazon.co.uk: Business, Industry &amp; Science</t>
-  </si>
-  <si>
-    <t>rudder</t>
-  </si>
-  <si>
-    <t>1 Pcs RC Boat Aluminium Alloy Brand New 75mm 95mm Metal Suction Water Rudder For Remote Control RC Boats CNC Upgrade Parts - AliExpress 26</t>
-  </si>
-  <si>
-    <t>motor couple 3.17-6mm</t>
-  </si>
-  <si>
-    <t>2mm/3mm/3.17mm/4mm/5mm/6mm/6.35mm/7mm/8mm/10mm Aluminum Rigid Shaft Coupler Rigid Coupling Motor Connector - AliExpress 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glue  </t>
-  </si>
-  <si>
-    <t>Plastic Glue 30 g, Clear Model Glue, Superglue for Plastic, Acrylic, Model, 3D Printing, Miniatures, PVC, Vinyl, with Anti-Clog Cap, Waterproof, Heat-Resistant : Amazon.co.uk: Home &amp; Kitchen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expanding foam </t>
-  </si>
-  <si>
-    <t>500ml Gap Expanding Foam Filler PU Expansion Insulation BONDING Filling - 1x : Amazon.co.uk: DIY &amp; Tools</t>
-  </si>
-  <si>
-    <t>prop set</t>
-  </si>
-  <si>
-    <t>1set 3.17mm 1/8" Flexible Cable Shaft + Shaft Sleeve + Mount Holder + 32mm Propeller Kit for RC Boats Marine Yacht - AliExpress 26</t>
+    <t>led</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Cree-LED/C566E-RFE-CV34QBB2?qs=sGAEpiMZZMusoohG2hS%252B1%2F8Ds1DTNiHJ2Y2ENDBgMaITswKiMImcrQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mfr Part Number </t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Mouser Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer Name</t>
+  </si>
+  <si>
+    <t>Quantity 1</t>
+  </si>
+  <si>
+    <t>Unit Price 1</t>
   </si>
 </sst>
 </file>
@@ -298,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,6 +434,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -655,20 +775,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:M28"/>
+  <dimension ref="B5:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="74" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="6" width="28.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.42578125" customWidth="1"/>
+    <col min="2" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" customWidth="1"/>
+    <col min="7" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="21" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:12">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -685,362 +806,507 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="42.75">
+    <row r="6" spans="2:12" ht="115.5">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>30.42</v>
-      </c>
-      <c r="E6" t="s">
+        <v>12.99</v>
+      </c>
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" ht="101.25">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>0.76</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="101.25">
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>8.99</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="J7" t="s">
         <v>10</v>
       </c>
-      <c r="M7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="42.75">
+      <c r="K7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="101.25">
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>2.99</v>
       </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="71.25">
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8">
+        <v>0.76</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="101.25">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>0.76</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="71.25">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="115.5">
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>0.76</v>
       </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="42.75">
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10">
+        <v>0.76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="115.5">
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>17.48</v>
       </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="71.25">
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>1.49</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="144.75">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C12">
         <v>0.76</v>
       </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" ht="71.25">
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12">
+        <v>3.99</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="87">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C13">
         <v>0.76</v>
       </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="57.75">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13">
+        <v>5.78</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="101.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>1.8</v>
       </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="71.25">
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14">
+        <v>11.06</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="115.5">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C15">
         <v>0.76</v>
       </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="71.25">
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15">
+        <v>0.13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="72.75">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C16">
         <v>0.76</v>
       </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16">
+        <v>0.24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="87">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>8.49</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="28.5">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17">
+        <v>1.64</v>
+      </c>
+      <c r="J17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="29.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C18">
         <v>20.49</v>
       </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18">
+        <v>1.33</v>
+      </c>
+      <c r="J18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C19">
         <v>12.55</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="87">
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20">
-        <v>0.76</v>
-      </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="72.75">
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21">
-        <v>9.7100000000000009</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="72.75">
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22">
-        <v>0.76</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="57.75">
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="72.75">
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24">
-        <v>0.76</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="72.75">
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25">
-        <v>1.49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="101.25">
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26">
-        <v>3.99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="57.75">
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27">
-        <v>5.78</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="72.75">
-      <c r="B28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28">
-        <v>11.06</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>57</v>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" t="s">
+        <v>88</v>
+      </c>
+      <c r="I19">
+        <v>0.111</v>
+      </c>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12"/>
+    <row r="21" spans="2:12"/>
+    <row r="22" spans="2:12"/>
+    <row r="23" spans="2:12"/>
+    <row r="24" spans="2:12"/>
+    <row r="25" spans="2:12"/>
+    <row r="26" spans="2:12"/>
+    <row r="27" spans="2:12"/>
+    <row r="28" spans="2:12"/>
+    <row r="29" spans="2:12"/>
+    <row r="30" spans="2:12"/>
+    <row r="31" spans="2:12"/>
+    <row r="42" spans="7:13" ht="15" customHeight="1">
+      <c r="G42" t="s">
+        <v>90</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L42" t="s">
+        <v>94</v>
+      </c>
+      <c r="M42" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1" xr:uid="{8288CBAE-7260-4A07-8E74-DF19B017B169}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{043AF1B3-0884-41A8-827B-42920022FFDB}"/>
-    <hyperlink ref="F11" r:id="rId3" xr:uid="{3381BD13-4897-4C3B-A7F1-57F58AE545BC}"/>
-    <hyperlink ref="F12" r:id="rId4" xr:uid="{BCB27762-8A88-4FA0-B229-A9CE4BD7C961}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{C9E7AAB0-299B-4A13-A1CD-B36F2684BC0A}"/>
-    <hyperlink ref="F13" r:id="rId6" xr:uid="{4385EB97-7CAE-42F8-81DA-F373F71DE2CC}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{FDAAFD89-E3C6-453E-8464-E78B7640EF6E}"/>
-    <hyperlink ref="F15" r:id="rId8" xr:uid="{86B149DE-B459-4162-9CBC-6324B618D3C9}"/>
-    <hyperlink ref="F18" r:id="rId9" xr:uid="{EC1F2CCB-FED4-4FD8-AF36-98F55C375756}"/>
-    <hyperlink ref="F19" r:id="rId10" display="https://www.amazon.co.uk/Tilswall-Quickly-Patents-Sealing-Repairs/dp/B07TD35L5R/ref=sr_1_1_sspa?crid=HOH2WAF927Y9&amp;dib=eyJ2IjoiMSJ9.U5hWFyJVy5RfGkY4q0pHCKc4nMrxit2RShdJQW1uVc3C2GDVF7l7cJztj_P51ZeDMaHy4Dx6tyZoBS0fHGihojy8bDc7vlQRrTUJ29bXtOQrqJGq-GG4qMe0v0EYdLBr1iKNh1BQZ1Tc7avCElQozLB1csy8apTDlK3Grt5ebvO8EqAtSPOrwEMjCq80BOjyx6gwxf032SYP5sE3e2hnyUF9MarSn4XofnWodu45kf6UvWp4vNl4uXq1nhcHFzC94reJ_SD1SIq6svRsvhTrdwoO5c3gEkgG_a_TaVzWau0.cov_Y0Lla9r2CHgGwHMme77sONmlGHg_mQKqe5GIr8U&amp;dib_tag=se&amp;keywords=glue%2Bgun&amp;qid=1747992083&amp;sprefix=glue%2Bgun%2B%2Caps%2C115&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1" xr:uid="{00AF2C7B-6C7A-4E0F-8190-21D4C567F4E6}"/>
-    <hyperlink ref="F17" r:id="rId11" display="https://www.amazon.co.uk/AmazonBasics-DS-SWP-Self-Adjusting-Wire-Stripper/dp/B07TS6KCXD/ref=sr_1_1_ffob_sspa?crid=4PXQPX64NXNF&amp;dib=eyJ2IjoiMSJ9.DH_EdmqxoPOOfvmEXfjH4Xq_PKbxWnzoBKytv_MODX4ZGDTjDm5t8YJGqj98qOJsQHa82X-Qpqu-LLlo806maEnUEzVc6kAK0mLmmo5JVqFyLElyaoTQI6srrh1CO6_06RjqEQRPdd4UObuIE3C2X-8txp_kqjh2M5ZhJgdd5pMpZU9fHxSdRlN3vxmi81QDNQtqPS-d1fAnphb1vf9iUtWMPeW1DQilRoim8ZN3BJ8.pN0LfIloJDcp6zmiOeLExXocUboft_UxQ_gaQTm-YZk&amp;dib_tag=se&amp;keywords=wire+strippers&amp;qid=1747992447&amp;s=diy&amp;sprefix=wire+s%2Cdiy%2C118&amp;sr=1-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{40D5ADB3-F70F-4A09-82B8-91A099956ED0}"/>
-    <hyperlink ref="F16" r:id="rId12" xr:uid="{7C2A9C0F-4F6A-431D-B04A-B8E7D7740B6D}"/>
-    <hyperlink ref="F7" r:id="rId13" xr:uid="{2BEF7346-CA44-47A0-8525-7930A49BE7C3}"/>
-    <hyperlink ref="F20" r:id="rId14" xr:uid="{4C655A12-777A-40E3-9B0F-49FD75FC3172}"/>
-    <hyperlink ref="F22" r:id="rId15" xr:uid="{3B9F1A94-451A-4787-8903-C0A210A9EF40}"/>
-    <hyperlink ref="F23" r:id="rId16" xr:uid="{FAB4B2ED-0633-4813-9D71-32E57C498B55}"/>
-    <hyperlink ref="F24" r:id="rId17" xr:uid="{B867861F-2722-46C6-8143-7C0AA698BDC5}"/>
-    <hyperlink ref="F25" r:id="rId18" xr:uid="{C4E8DB09-EDA3-4F83-A009-B5B8A6294A0D}"/>
-    <hyperlink ref="F26" r:id="rId19" xr:uid="{1EB7E4F0-48D9-40F5-BE5C-E97AF9BECF35}"/>
-    <hyperlink ref="F27" r:id="rId20" xr:uid="{DA4A9DEC-5B7F-4D49-9704-1A9EB0891B17}"/>
-    <hyperlink ref="F28" r:id="rId21" xr:uid="{F67153BD-6596-47F5-8FA5-638C2DB6E95D}"/>
-    <hyperlink ref="F21" r:id="rId22" xr:uid="{798A221E-271E-43A5-B608-6B687CDD18A8}"/>
-    <hyperlink ref="F14" r:id="rId23" xr:uid="{1CF0676A-CF93-48C7-AA96-7C6F647143EC}"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{043AF1B3-0884-41A8-827B-42920022FFDB}"/>
+    <hyperlink ref="E11" r:id="rId2" xr:uid="{3381BD13-4897-4C3B-A7F1-57F58AE545BC}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{BCB27762-8A88-4FA0-B229-A9CE4BD7C961}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{C9E7AAB0-299B-4A13-A1CD-B36F2684BC0A}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{4385EB97-7CAE-42F8-81DA-F373F71DE2CC}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{FDAAFD89-E3C6-453E-8464-E78B7640EF6E}"/>
+    <hyperlink ref="E15" r:id="rId7" xr:uid="{86B149DE-B459-4162-9CBC-6324B618D3C9}"/>
+    <hyperlink ref="E18" r:id="rId8" xr:uid="{EC1F2CCB-FED4-4FD8-AF36-98F55C375756}"/>
+    <hyperlink ref="E19" r:id="rId9" display="https://www.amazon.co.uk/Tilswall-Quickly-Patents-Sealing-Repairs/dp/B07TD35L5R/ref=sr_1_1_sspa?crid=HOH2WAF927Y9&amp;dib=eyJ2IjoiMSJ9.U5hWFyJVy5RfGkY4q0pHCKc4nMrxit2RShdJQW1uVc3C2GDVF7l7cJztj_P51ZeDMaHy4Dx6tyZoBS0fHGihojy8bDc7vlQRrTUJ29bXtOQrqJGq-GG4qMe0v0EYdLBr1iKNh1BQZ1Tc7avCElQozLB1csy8apTDlK3Grt5ebvO8EqAtSPOrwEMjCq80BOjyx6gwxf032SYP5sE3e2hnyUF9MarSn4XofnWodu45kf6UvWp4vNl4uXq1nhcHFzC94reJ_SD1SIq6svRsvhTrdwoO5c3gEkgG_a_TaVzWau0.cov_Y0Lla9r2CHgGwHMme77sONmlGHg_mQKqe5GIr8U&amp;dib_tag=se&amp;keywords=glue%2Bgun&amp;qid=1747992083&amp;sprefix=glue%2Bgun%2B%2Caps%2C115&amp;sr=8-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;th=1" xr:uid="{00AF2C7B-6C7A-4E0F-8190-21D4C567F4E6}"/>
+    <hyperlink ref="E17" r:id="rId10" display="https://www.amazon.co.uk/AmazonBasics-DS-SWP-Self-Adjusting-Wire-Stripper/dp/B07TS6KCXD/ref=sr_1_1_ffob_sspa?crid=4PXQPX64NXNF&amp;dib=eyJ2IjoiMSJ9.DH_EdmqxoPOOfvmEXfjH4Xq_PKbxWnzoBKytv_MODX4ZGDTjDm5t8YJGqj98qOJsQHa82X-Qpqu-LLlo806maEnUEzVc6kAK0mLmmo5JVqFyLElyaoTQI6srrh1CO6_06RjqEQRPdd4UObuIE3C2X-8txp_kqjh2M5ZhJgdd5pMpZU9fHxSdRlN3vxmi81QDNQtqPS-d1fAnphb1vf9iUtWMPeW1DQilRoim8ZN3BJ8.pN0LfIloJDcp6zmiOeLExXocUboft_UxQ_gaQTm-YZk&amp;dib_tag=se&amp;keywords=wire+strippers&amp;qid=1747992447&amp;s=diy&amp;sprefix=wire+s%2Cdiy%2C118&amp;sr=1-1-spons&amp;sp_csd=d2lkZ2V0TmFtZT1zcF9hdGY&amp;psc=1" xr:uid="{40D5ADB3-F70F-4A09-82B8-91A099956ED0}"/>
+    <hyperlink ref="E16" r:id="rId11" xr:uid="{7C2A9C0F-4F6A-431D-B04A-B8E7D7740B6D}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{2BEF7346-CA44-47A0-8525-7930A49BE7C3}"/>
+    <hyperlink ref="K6" r:id="rId13" xr:uid="{4C655A12-777A-40E3-9B0F-49FD75FC3172}"/>
+    <hyperlink ref="K8" r:id="rId14" xr:uid="{3B9F1A94-451A-4787-8903-C0A210A9EF40}"/>
+    <hyperlink ref="K9" r:id="rId15" xr:uid="{FAB4B2ED-0633-4813-9D71-32E57C498B55}"/>
+    <hyperlink ref="K10" r:id="rId16" xr:uid="{B867861F-2722-46C6-8143-7C0AA698BDC5}"/>
+    <hyperlink ref="K11" r:id="rId17" xr:uid="{C4E8DB09-EDA3-4F83-A009-B5B8A6294A0D}"/>
+    <hyperlink ref="K12" r:id="rId18" xr:uid="{1EB7E4F0-48D9-40F5-BE5C-E97AF9BECF35}"/>
+    <hyperlink ref="K13" r:id="rId19" xr:uid="{DA4A9DEC-5B7F-4D49-9704-1A9EB0891B17}"/>
+    <hyperlink ref="K14" r:id="rId20" xr:uid="{F67153BD-6596-47F5-8FA5-638C2DB6E95D}"/>
+    <hyperlink ref="K7" r:id="rId21" xr:uid="{798A221E-271E-43A5-B608-6B687CDD18A8}"/>
+    <hyperlink ref="E14" r:id="rId22" xr:uid="{1CF0676A-CF93-48C7-AA96-7C6F647143EC}"/>
+    <hyperlink ref="E6" r:id="rId23" xr:uid="{63FEFB20-7376-43DF-86F1-2706A0E83767}"/>
+    <hyperlink ref="K18" r:id="rId24" xr:uid="{4DE8FB65-55E3-4F60-8DAD-72BEC2230D67}"/>
+    <hyperlink ref="K17" r:id="rId25" xr:uid="{F51D90C8-3B21-4B22-9F45-77C4F50A366E}"/>
+    <hyperlink ref="K19" r:id="rId26" xr:uid="{F2A63475-5EA8-462B-AAD5-387582F238A2}"/>
+    <hyperlink ref="K16" r:id="rId27" xr:uid="{8A4FBE77-8472-4438-B7B8-B1ADD14DEFDD}"/>
+    <hyperlink ref="K15" r:id="rId28" xr:uid="{47AB8318-DDE6-4DF9-BDA4-221BA4FDB1A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>